<commit_message>
Add Bloomberg workbook automation and document export data
</commit_message>
<xml_diff>
--- a/data/bloomberg/raw/bloomberg_export_72assets.xlsx
+++ b/data/bloomberg/raw/bloomberg_export_72assets.xlsx
@@ -433,7 +433,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F76"/>
+  <dimension ref="A1:F70"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -475,7 +475,7 @@
         </is>
       </c>
       <c r="F1">
-        <f>BDH($D$2:$D$76,"PX_LAST","19900101","20251116","Dir=V")</f>
+        <f>BDH($D$2:$D$70,"PX_LAST","19900101","20251116","Dir=V")</f>
         <v/>
       </c>
     </row>
@@ -1994,34 +1994,34 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t># Note: VG1</t>
+          <t>GX</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Z 1</t>
+          <t>EQ</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t xml:space="preserve"> NK1 already in dataset as XX/XU</t>
+          <t>DAX Index</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t xml:space="preserve"> LX</t>
+          <t>GX1 Index</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t xml:space="preserve"> NK</t>
+          <t>Eurex DAX - German equity benchmark. Euro-denominated</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>GX</t>
+          <t>TP</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -2031,24 +2031,24 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>DAX Index</t>
+          <t>TOPIX Index</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>GX1 Index</t>
+          <t>TP1 Index</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>Eurex DAX - German equity benchmark. Euro-denominated</t>
+          <t>JPX TOPIX - broader Japan market vs NK (Nikkei 225)</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>TP</t>
+          <t>HI</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -2058,24 +2058,24 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>TOPIX Index</t>
+          <t>Hang Seng Index</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>TP1 Index</t>
+          <t>HI1 Index</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>JPX TOPIX - broader Japan market vs NK (Nikkei 225)</t>
+          <t>HKEX Hang Seng - Hong Kong/China exposure</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>HI</t>
+          <t>TS</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -2085,51 +2085,51 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Hang Seng Index</t>
+          <t>FTSE/JSE Top 40</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>HI1 Index</t>
+          <t>ZTSA Index</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>HKEX Hang Seng - Hong Kong/China exposure</t>
+          <t>JSE South Africa Top 40 - emerging market equity</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>TS</t>
+          <t>BC</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>EQ</t>
+          <t>CR</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>FTSE/JSE Top 40</t>
+          <t>Bitcoin (aggregate)</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>ZTSA Index</t>
+          <t>BTCA Curncy</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>JSE South Africa Top 40 - emerging market equity</t>
+          <t>Bitcoin aggregate index - crypto flagship</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>BC</t>
+          <t>DC</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -2139,24 +2139,24 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Bitcoin (aggregate)</t>
+          <t>Decred</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>BTCA Curncy</t>
+          <t>DCRA Curncy</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>Bitcoin aggregate index - crypto flagship</t>
+          <t>Decred aggregate - alt L1 blockchain</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>DC</t>
+          <t>XM</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -2166,24 +2166,24 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Decred</t>
+          <t>Monero</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>DCRA Curncy</t>
+          <t>MERA Curncy</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>Decred aggregate - alt L1 blockchain</t>
+          <t>Monero aggregate - privacy coin</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>XM</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -2193,105 +2193,105 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Monero</t>
+          <t>Bitcoin Cash</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>MERA Curncy</t>
+          <t>BMR Curncy</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>Monero aggregate - privacy coin</t>
+          <t>Bitcoin Cash - Bitcoin fork</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>XAU</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>CR</t>
+          <t>SP</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Bitcoin Cash</t>
+          <t>Gold Spot vs USD</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>BMR Curncy</t>
+          <t>XAUUSD Curncy</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>Bitcoin Cash - Bitcoin fork</t>
+          <t>Spot gold - basis vs ZG futures. London fix reference</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t># SO</t>
+          <t>XAG</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>CR</t>
+          <t>SP</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Solana</t>
+          <t>Silver Spot vs USD</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>&lt;TBD&gt; Curncy</t>
+          <t>XAGUSD Curncy</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>CME Solana - to be confirmed from CME vendor file</t>
+          <t>Spot silver - basis vs ZI futures</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t># XR</t>
+          <t>XPT</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>CR</t>
+          <t>SP</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Ripple (XRP)</t>
+          <t>Platinum Spot vs USD</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>&lt;TBD&gt; Curncy</t>
+          <t>XPTUSD Curncy</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>CME XRP - to be confirmed from CME vendor file</t>
+          <t>Spot platinum - basis vs ZP futures</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>XAU</t>
+          <t>XPD</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -2301,191 +2301,44 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Gold Spot vs USD</t>
+          <t>Palladium Spot vs USD</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>XAUUSD Curncy</t>
+          <t>XPDUSD Curncy</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>Spot gold - basis vs ZG futures. London fix reference</t>
+          <t>Spot palladium - basis vs ZA futures</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>XAG</t>
+          <t>RB</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>SP</t>
+          <t>CM</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Silver Spot vs USD</t>
+          <t>RBOB Gasoline</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>XAGUSD Curncy</t>
+          <t>XB1 Comdty</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>Spot silver - basis vs ZI futures</t>
-        </is>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" t="inlineStr">
-        <is>
-          <t>XPT</t>
-        </is>
-      </c>
-      <c r="B71" t="inlineStr">
-        <is>
-          <t>SP</t>
-        </is>
-      </c>
-      <c r="C71" t="inlineStr">
-        <is>
-          <t>Platinum Spot vs USD</t>
-        </is>
-      </c>
-      <c r="D71" t="inlineStr">
-        <is>
-          <t>XPTUSD Curncy</t>
-        </is>
-      </c>
-      <c r="E71" t="inlineStr">
-        <is>
-          <t>Spot platinum - basis vs ZP futures</t>
-        </is>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="inlineStr">
-        <is>
-          <t>XPD</t>
-        </is>
-      </c>
-      <c r="B72" t="inlineStr">
-        <is>
-          <t>SP</t>
-        </is>
-      </c>
-      <c r="C72" t="inlineStr">
-        <is>
-          <t>Palladium Spot vs USD</t>
-        </is>
-      </c>
-      <c r="D72" t="inlineStr">
-        <is>
-          <t>XPDUSD Curncy</t>
-        </is>
-      </c>
-      <c r="E72" t="inlineStr">
-        <is>
-          <t>Spot palladium - basis vs ZA futures</t>
-        </is>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="inlineStr">
-        <is>
-          <t>RB</t>
-        </is>
-      </c>
-      <c r="B73" t="inlineStr">
-        <is>
-          <t>CM</t>
-        </is>
-      </c>
-      <c r="C73" t="inlineStr">
-        <is>
-          <t>RBOB Gasoline</t>
-        </is>
-      </c>
-      <c r="D73" t="inlineStr">
-        <is>
-          <t>XB1 Comdty</t>
-        </is>
-      </c>
-      <c r="E73" t="inlineStr">
-        <is>
           <t>NYMEX RBOB - gasoline crack spread vs crude oil (ZU)</t>
-        </is>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="inlineStr">
-        <is>
-          <t># Global indices (4): DAX</t>
-        </is>
-      </c>
-      <c r="B74" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> TOPIX</t>
-        </is>
-      </c>
-      <c r="C74" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Hang Seng</t>
-        </is>
-      </c>
-      <c r="D74" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> JSE Top 40</t>
-        </is>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="inlineStr">
-        <is>
-          <t># Crypto (4+2): BTC</t>
-        </is>
-      </c>
-      <c r="B75" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> DCR</t>
-        </is>
-      </c>
-      <c r="C75" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> XMR</t>
-        </is>
-      </c>
-      <c r="D75" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> BCH + pending SOL/XRP</t>
-        </is>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" t="inlineStr">
-        <is>
-          <t># Spot metals (4): XAU</t>
-        </is>
-      </c>
-      <c r="B76" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> XAG</t>
-        </is>
-      </c>
-      <c r="C76" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> XPT</t>
-        </is>
-      </c>
-      <c r="D76" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> XPD vs futures basis</t>
         </is>
       </c>
     </row>

</xml_diff>